<commit_message>
Check aj2 and dd1 blind counts
</commit_message>
<xml_diff>
--- a/original/EE_counts_DD.xlsx
+++ b/original/EE_counts_DD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/early_experience/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DB790B0-CB48-4D4B-98A4-F771FA3FA8B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D8F29-2A75-E246-95FA-4CE267D886DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6680" yWindow="460" windowWidth="17680" windowHeight="16240" xr2:uid="{3C7FC68B-35C2-1944-A911-FDD3EAD98C36}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>image_id</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>not sure</t>
-  </si>
-  <si>
-    <t>?3</t>
   </si>
   <si>
     <t>blurry</t>
@@ -420,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70EA5A4F-1F9A-2E4E-82C7-55D13603B165}">
   <dimension ref="A1:C275"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,7 +442,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,8 +1567,8 @@
       <c r="A139">
         <v>15700</v>
       </c>
-      <c r="B139" t="s">
-        <v>11</v>
+      <c r="B139">
+        <v>3</v>
       </c>
       <c r="C139" t="s">
         <v>10</v>
@@ -1753,7 +1750,7 @@
         <v>6</v>
       </c>
       <c r="C161" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
correct a recycled nadom# in name_conversion.txt
</commit_message>
<xml_diff>
--- a/original/EE_counts_DD.xlsx
+++ b/original/EE_counts_DD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngomae/MyGithub/early_experience/original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D8F29-2A75-E246-95FA-4CE267D886DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86220EE-438A-1649-B511-7051DCDB723E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6680" yWindow="460" windowWidth="17680" windowHeight="16240" xr2:uid="{3C7FC68B-35C2-1944-A911-FDD3EAD98C36}"/>
+    <workbookView xWindow="3940" yWindow="3460" windowWidth="22820" windowHeight="16240" xr2:uid="{3C7FC68B-35C2-1944-A911-FDD3EAD98C36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70EA5A4F-1F9A-2E4E-82C7-55D13603B165}">
   <dimension ref="A1:C275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124:XFD124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,18 +1624,18 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>16527</v>
+        <v>16523</v>
       </c>
       <c r="B146">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>16523</v>
+        <v>16527</v>
       </c>
       <c r="B147">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,90 +1995,90 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192">
-        <v>26373</v>
+        <v>23786</v>
       </c>
       <c r="B192">
-        <v>180</v>
+        <v>75</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193">
-        <v>23786</v>
+        <v>23984</v>
       </c>
       <c r="B193">
-        <v>75</v>
+        <v>42</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194">
-        <v>23984</v>
+        <v>24191</v>
       </c>
       <c r="B194">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195">
-        <v>24191</v>
+        <v>24601</v>
       </c>
       <c r="B195">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196">
-        <v>24601</v>
+        <v>24710</v>
       </c>
       <c r="B196">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>24710</v>
+        <v>24844</v>
       </c>
       <c r="B197">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198">
-        <v>24844</v>
+        <v>24882</v>
       </c>
       <c r="B198">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199">
-        <v>24882</v>
+        <v>24917</v>
       </c>
       <c r="B199">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200">
-        <v>24917</v>
+        <v>24941</v>
       </c>
       <c r="B200">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201">
-        <v>24941</v>
+        <v>24972</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202">
-        <v>24972</v>
+        <v>25100</v>
       </c>
       <c r="B202">
-        <v>270</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
@@ -2091,98 +2091,98 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>25100</v>
+        <v>25114</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>378</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205">
-        <v>25114</v>
+        <v>25150</v>
       </c>
       <c r="B205">
-        <v>378</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206">
-        <v>25150</v>
+        <v>25219</v>
       </c>
       <c r="B206">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207">
-        <v>25219</v>
+        <v>25250</v>
       </c>
       <c r="B207">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208">
-        <v>25250</v>
+        <v>25329</v>
       </c>
       <c r="B208">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209">
-        <v>25329</v>
+        <v>25429</v>
       </c>
       <c r="B209">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210">
-        <v>25429</v>
+        <v>25659</v>
       </c>
       <c r="B210">
-        <v>13</v>
+        <v>225</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211">
-        <v>25659</v>
+        <v>25664</v>
       </c>
       <c r="B211">
-        <v>225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212">
-        <v>25664</v>
+        <v>26068</v>
       </c>
       <c r="B212">
-        <v>0</v>
+        <v>501</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213">
-        <v>26068</v>
+        <v>26179</v>
       </c>
       <c r="B213">
-        <v>501</v>
+        <v>6</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214">
-        <v>26179</v>
+        <v>26220</v>
       </c>
       <c r="B214">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215">
-        <v>26220</v>
+        <v>26373</v>
       </c>
       <c r="B215">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
@@ -2669,6 +2669,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C275">
+    <sortCondition ref="A2:A275"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>